<commit_message>
Se agrego los modelos: provvedor, categoria, historial de ventas se areglo el metodo guardar datos se arrglo el metodo leer excel se complilo en prueba para verficar
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\Sistema de almacen\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{418137DF-E5EC-4386-BD6C-6C683AA0A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD8E62-9CCA-49BA-BB9E-006EAD1C5E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4E2ADF9C-5ABC-4121-9AC5-090A39F36A55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4E2ADF9C-5ABC-4121-9AC5-090A39F36A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
     <sheet name="Usuarios" sheetId="2" r:id="rId2"/>
+    <sheet name="Categorias" sheetId="3" r:id="rId3"/>
+    <sheet name="Proveedores" sheetId="4" r:id="rId4"/>
+    <sheet name="HistorialVentas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="79">
   <si>
     <t>codigo</t>
   </si>
@@ -97,9 +100,6 @@
     <t>PROV-B</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>PROD-003</t>
   </si>
   <si>
@@ -206,6 +206,75 @@
   </si>
   <si>
     <t>Prov-0045</t>
+  </si>
+  <si>
+    <t>nombreCategoria</t>
+  </si>
+  <si>
+    <t>Lácteos</t>
+  </si>
+  <si>
+    <t>Abarrotes</t>
+  </si>
+  <si>
+    <t>Bebidas</t>
+  </si>
+  <si>
+    <t>Conservas</t>
+  </si>
+  <si>
+    <t>Limpieza</t>
+  </si>
+  <si>
+    <t>idVenta</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>productoVendido</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>VENTA-001</t>
+  </si>
+  <si>
+    <t>VENTA-002</t>
+  </si>
+  <si>
+    <t>Distribuidora Central S.A.</t>
+  </si>
+  <si>
+    <t>Alicorp S.A.A.</t>
+  </si>
+  <si>
+    <t>Arca Continental Lindley</t>
+  </si>
+  <si>
+    <t>idProveedor (int)</t>
+  </si>
+  <si>
+    <t>nombre (String)</t>
+  </si>
+  <si>
+    <t>telefono (String)</t>
+  </si>
+  <si>
+    <t>email (String)</t>
+  </si>
+  <si>
+    <t>ventas@central.com</t>
+  </si>
+  <si>
+    <t>contacto@alicorp.pe</t>
+  </si>
+  <si>
+    <t>pedidos@arca.com</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -245,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -260,32 +329,6 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -329,115 +372,37 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -583,13 +548,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -599,6 +557,13 @@
         <top style="medium">
           <color rgb="FF000000"/>
         </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
@@ -632,25 +597,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
       <font>
@@ -1007,13 +953,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -1026,6 +965,61 @@
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1042,32 +1036,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DE182EC-393B-425D-9A86-F973FE66AD62}" name="Tabla1" displayName="Tabla1" ref="A1:J7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9" headerRowBorderDxfId="21" tableBorderDxfId="22" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DE182EC-393B-425D-9A86-F973FE66AD62}" name="Tabla1" displayName="Tabla1" ref="A1:J7" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A1:J7" xr:uid="{9DE182EC-393B-425D-9A86-F973FE66AD62}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A86C56FD-2CAA-4503-8706-DE6BF1E15690}" name="codigo" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{94D78787-A3C7-42EB-8499-D502E751CF6B}" name="nombre" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{CB7B0577-1E99-458B-B4F4-8B8F510066F1}" name="descripcion" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{956BF0D9-5FF8-4956-B33A-DFC75670164D}" name="precioCompra" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{55900EF7-7B93-4C71-862C-E4DF7AAF1BA6}" name="precioVenta" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{6E31B920-1938-4064-8A8B-B9766AB94DF2}" name="stock" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{C291AAED-AFD7-40DB-BDCE-2655A373C7FE}" name="stockMinimo" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{25AB14AC-EBCD-4A79-837F-24518BFBC13F}" name="idCategoria" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{266051CB-C652-4123-97C0-1BCD68598E97}" name="idProveedor" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{233C4657-ADC3-4AEE-A6E4-88BFD354C053}" name="fechaVencimiento" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{A86C56FD-2CAA-4503-8706-DE6BF1E15690}" name="codigo" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{94D78787-A3C7-42EB-8499-D502E751CF6B}" name="nombre" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{CB7B0577-1E99-458B-B4F4-8B8F510066F1}" name="descripcion" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{956BF0D9-5FF8-4956-B33A-DFC75670164D}" name="precioCompra" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{55900EF7-7B93-4C71-862C-E4DF7AAF1BA6}" name="precioVenta" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{6E31B920-1938-4064-8A8B-B9766AB94DF2}" name="stock" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{C291AAED-AFD7-40DB-BDCE-2655A373C7FE}" name="stockMinimo" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{25AB14AC-EBCD-4A79-837F-24518BFBC13F}" name="idCategoria" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{266051CB-C652-4123-97C0-1BCD68598E97}" name="idProveedor" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{233C4657-ADC3-4AEE-A6E4-88BFD354C053}" name="fechaVencimiento" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9E755E2-12CC-4510-A781-E50E8C326364}" name="Tabla2" displayName="Tabla2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9E755E2-12CC-4510-A781-E50E8C326364}" name="Tabla2" displayName="Tabla2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:D4" xr:uid="{C9E755E2-12CC-4510-A781-E50E8C326364}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{475C9F48-CDC2-4883-9B95-D3B79C76F66A}" name="idUsuario" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{CE27346D-1DB5-4098-AB9E-EC5CD38449F2}" name="nombreUsuario" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E01CC466-357B-455C-B857-AE83DA79C7DA}" name="contrasena" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B896747C-FB98-434E-95B2-0327AAFDCC54}" name="rol" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{475C9F48-CDC2-4883-9B95-D3B79C76F66A}" name="idUsuario" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CE27346D-1DB5-4098-AB9E-EC5CD38449F2}" name="nombreUsuario" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E01CC466-357B-455C-B857-AE83DA79C7DA}" name="contrasena" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B896747C-FB98-434E-95B2-0327AAFDCC54}" name="rol" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1370,7 +1364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012D4005-2E5B-4316-B331-8FBB6649AB07}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -1389,34 +1383,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1448,7 +1442,7 @@
       <c r="I2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="J2" t="n" s="14">
+      <c r="J2" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1484,13 +1478,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s" s="0">
         <v>22</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>23</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>8.0</v>
@@ -1514,13 +1508,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="C5" t="s" s="0">
         <v>25</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>26</v>
       </c>
       <c r="D5" t="n" s="0">
         <v>6.5</v>
@@ -1535,24 +1529,24 @@
         <v>10.0</v>
       </c>
       <c r="H5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="I5" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J5" t="n" s="14">
+      <c r="J5" t="n" s="8">
         <v>45838.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="C6" t="s" s="0">
         <v>30</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>31</v>
       </c>
       <c r="D6" t="n" s="0">
         <v>5.0</v>
@@ -1567,24 +1561,24 @@
         <v>25.0</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="J6" t="n" s="14">
+      <c r="J6" t="n" s="8">
         <v>46387.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="C7" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>35</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>12.0</v>
@@ -1599,7 +1593,7 @@
         <v>5.0</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s" s="0">
         <v>14</v>
@@ -1608,13 +1602,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="C8" t="s" s="0">
         <v>53</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>54</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>99.39</v>
@@ -1629,24 +1623,24 @@
         <v>2.0</v>
       </c>
       <c r="H8" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="I8" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="J8" t="n" s="14">
+      <c r="J8" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="C9" t="s" s="0">
         <v>53</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>54</v>
       </c>
       <c r="D9" t="n" s="0">
         <v>99.39</v>
@@ -1661,24 +1655,24 @@
         <v>2.0</v>
       </c>
       <c r="H9" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="I9" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="J9" t="n" s="14">
+      <c r="J9" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="C10" t="s" s="0">
         <v>53</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>54</v>
       </c>
       <c r="D10" t="n" s="0">
         <v>99.39</v>
@@ -1693,24 +1687,24 @@
         <v>2.0</v>
       </c>
       <c r="H10" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="I10" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="J10" t="n" s="14">
+      <c r="J10" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="C11" t="s" s="0">
         <v>53</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>54</v>
       </c>
       <c r="D11" t="n" s="0">
         <v>99.39</v>
@@ -1725,12 +1719,76 @@
         <v>2.0</v>
       </c>
       <c r="H11" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I11" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="I11" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="J11" t="n" s="14">
+      <c r="J11" t="n" s="8">
+        <v>46022.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>99.39</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>101.2</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="G12" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J12" t="n" s="8">
+        <v>46022.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>99.39</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>101.2</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="G13" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J13" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1744,9 +1802,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348FFC53-07F3-4ABC-B1C5-CEEA266BDD53}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1758,59 +1816,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>44</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1819,4 +1875,182 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E73D91-ABA1-4E4F-B8D2-1667158F783C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7073E4-1EA7-4177-B7B7-C33464062EA9}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="16.6640625"/>
+    <col min="3" max="3" customWidth="true" width="20.33203125"/>
+    <col min="4" max="4" customWidth="true" width="23.5546875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>9.87654321E8</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>9.99888777E8</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>9.12345678E8</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF12A230-5A23-46F0-BF7B-670F7DECCE22}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="20.109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B2" t="n" s="8">
+        <v>45951.0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B3" t="n" s="8">
+        <v>45951.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>8.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se corrigio el metodo excel debido a un error
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\Sistema de almacen\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD8E62-9CCA-49BA-BB9E-006EAD1C5E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF6F16-65B1-4384-8E41-8BCA54ED8DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4E2ADF9C-5ABC-4121-9AC5-090A39F36A55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{4E2ADF9C-5ABC-4121-9AC5-090A39F36A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="79">
   <si>
     <t>codigo</t>
   </si>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -394,15 +394,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -425,7 +441,416 @@
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
         <right/>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
         <top style="medium">
           <color rgb="FF000000"/>
         </top>
@@ -563,6 +988,25 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1B1C1D"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color rgb="FF000000"/>
@@ -598,430 +1042,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF1B1C1D"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1036,32 +1056,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DE182EC-393B-425D-9A86-F973FE66AD62}" name="Tabla1" displayName="Tabla1" ref="A1:J7" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DE182EC-393B-425D-9A86-F973FE66AD62}" name="Tabla1" displayName="Tabla1" ref="A1:J7" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:J7" xr:uid="{9DE182EC-393B-425D-9A86-F973FE66AD62}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A86C56FD-2CAA-4503-8706-DE6BF1E15690}" name="codigo" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{94D78787-A3C7-42EB-8499-D502E751CF6B}" name="nombre" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{CB7B0577-1E99-458B-B4F4-8B8F510066F1}" name="descripcion" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{956BF0D9-5FF8-4956-B33A-DFC75670164D}" name="precioCompra" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{55900EF7-7B93-4C71-862C-E4DF7AAF1BA6}" name="precioVenta" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{6E31B920-1938-4064-8A8B-B9766AB94DF2}" name="stock" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{C291AAED-AFD7-40DB-BDCE-2655A373C7FE}" name="stockMinimo" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{25AB14AC-EBCD-4A79-837F-24518BFBC13F}" name="idCategoria" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{266051CB-C652-4123-97C0-1BCD68598E97}" name="idProveedor" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{233C4657-ADC3-4AEE-A6E4-88BFD354C053}" name="fechaVencimiento" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{A86C56FD-2CAA-4503-8706-DE6BF1E15690}" name="codigo" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{94D78787-A3C7-42EB-8499-D502E751CF6B}" name="nombre" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{CB7B0577-1E99-458B-B4F4-8B8F510066F1}" name="descripcion" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{956BF0D9-5FF8-4956-B33A-DFC75670164D}" name="precioCompra" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{55900EF7-7B93-4C71-862C-E4DF7AAF1BA6}" name="precioVenta" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{6E31B920-1938-4064-8A8B-B9766AB94DF2}" name="stock" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{C291AAED-AFD7-40DB-BDCE-2655A373C7FE}" name="stockMinimo" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{25AB14AC-EBCD-4A79-837F-24518BFBC13F}" name="idCategoria" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{266051CB-C652-4123-97C0-1BCD68598E97}" name="idProveedor" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{233C4657-ADC3-4AEE-A6E4-88BFD354C053}" name="fechaVencimiento" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9E755E2-12CC-4510-A781-E50E8C326364}" name="Tabla2" displayName="Tabla2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9E755E2-12CC-4510-A781-E50E8C326364}" name="Tabla2" displayName="Tabla2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:D4" xr:uid="{C9E755E2-12CC-4510-A781-E50E8C326364}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{475C9F48-CDC2-4883-9B95-D3B79C76F66A}" name="idUsuario" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{CE27346D-1DB5-4098-AB9E-EC5CD38449F2}" name="nombreUsuario" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{E01CC466-357B-455C-B857-AE83DA79C7DA}" name="contrasena" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B896747C-FB98-434E-95B2-0327AAFDCC54}" name="rol" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{475C9F48-CDC2-4883-9B95-D3B79C76F66A}" name="idUsuario" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{CE27346D-1DB5-4098-AB9E-EC5CD38449F2}" name="nombreUsuario" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{E01CC466-357B-455C-B857-AE83DA79C7DA}" name="contrasena" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B896747C-FB98-434E-95B2-0327AAFDCC54}" name="rol" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1364,7 +1384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012D4005-2E5B-4316-B331-8FBB6649AB07}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -1442,7 +1462,7 @@
       <c r="I2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="J2" t="n" s="8">
+      <c r="J2" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1534,7 +1554,7 @@
       <c r="I5" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="J5" t="n" s="8">
+      <c r="J5" t="n" s="7">
         <v>45838.0</v>
       </c>
     </row>
@@ -1566,7 +1586,7 @@
       <c r="I6" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="J6" t="n" s="8">
+      <c r="J6" t="n" s="7">
         <v>46387.0</v>
       </c>
     </row>
@@ -1628,7 +1648,7 @@
       <c r="I8" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J8" t="n" s="8">
+      <c r="J8" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1660,7 +1680,7 @@
       <c r="I9" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J9" t="n" s="8">
+      <c r="J9" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1692,7 +1712,7 @@
       <c r="I10" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J10" t="n" s="8">
+      <c r="J10" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1724,7 +1744,7 @@
       <c r="I11" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J11" t="n" s="8">
+      <c r="J11" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1756,7 +1776,7 @@
       <c r="I12" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J12" t="n" s="8">
+      <c r="J12" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1788,7 +1808,39 @@
       <c r="I13" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J13" t="n" s="8">
+      <c r="J13" t="n" s="7">
+        <v>46022.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>99.39</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>101.2</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J14" t="n" s="7">
         <v>46022.0</v>
       </c>
     </row>
@@ -1802,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348FFC53-07F3-4ABC-B1C5-CEEA266BDD53}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1831,42 +1883,44 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1879,13 +1933,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E73D91-ABA1-4E4F-B8D2-1667158F783C}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="15.0"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
@@ -1893,6 +1951,46 @@
       </c>
       <c r="B1" s="6" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +2003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7073E4-1EA7-4177-B7B7-C33464062EA9}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1981,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF12A230-5A23-46F0-BF7B-670F7DECCE22}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,7 +2112,7 @@
       <c r="A2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B2" t="n" s="8">
+      <c r="B2" t="n" s="7">
         <v>45951.0</v>
       </c>
       <c r="C2" t="s" s="0">
@@ -2034,7 +2132,7 @@
       <c r="A3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B3" t="n" s="8">
+      <c r="B3" t="n" s="7">
         <v>45951.0</v>
       </c>
       <c r="C3" t="s" s="0">

</xml_diff>

<commit_message>
se hizo una interface para simplificar los metodos se hizo uba caopeta metodos para nas orden se agregaron imagenes se hizo el CRUD de usuarios se hizo el formulario login, gestionar usuarios, principal
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="79">
   <si>
     <t>codigo</t>
   </si>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -394,6 +394,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1384,7 +1385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012D4005-2E5B-4316-B331-8FBB6649AB07}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -1462,7 +1463,7 @@
       <c r="I2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="J2" t="n" s="7">
+      <c r="J2" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1554,7 +1555,7 @@
       <c r="I5" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="J5" t="n" s="7">
+      <c r="J5" t="n" s="8">
         <v>45838.0</v>
       </c>
     </row>
@@ -1586,7 +1587,7 @@
       <c r="I6" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="J6" t="n" s="7">
+      <c r="J6" t="n" s="8">
         <v>46387.0</v>
       </c>
     </row>
@@ -1648,7 +1649,7 @@
       <c r="I8" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J8" t="n" s="7">
+      <c r="J8" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1680,7 +1681,7 @@
       <c r="I9" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J9" t="n" s="7">
+      <c r="J9" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1712,7 +1713,7 @@
       <c r="I10" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J10" t="n" s="7">
+      <c r="J10" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1744,7 +1745,7 @@
       <c r="I11" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J11" t="n" s="7">
+      <c r="J11" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1776,7 +1777,7 @@
       <c r="I12" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J12" t="n" s="7">
+      <c r="J12" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1808,7 +1809,7 @@
       <c r="I13" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J13" t="n" s="7">
+      <c r="J13" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -1840,7 +1841,39 @@
       <c r="I14" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J14" t="n" s="7">
+      <c r="J14" t="n" s="8">
+        <v>46022.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>99.39</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>101.2</v>
+      </c>
+      <c r="F15" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="G15" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J15" t="n" s="8">
         <v>46022.0</v>
       </c>
     </row>
@@ -2112,7 +2145,7 @@
       <c r="A2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B2" t="n" s="7">
+      <c r="B2" t="n" s="8">
         <v>45951.0</v>
       </c>
       <c r="C2" t="s" s="0">
@@ -2132,7 +2165,7 @@
       <c r="A3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B3" t="n" s="7">
+      <c r="B3" t="n" s="8">
         <v>45951.0</v>
       </c>
       <c r="C3" t="s" s="0">

</xml_diff>

<commit_message>
se agregaron los metodos del integrnte 5
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="79">
   <si>
     <t>codigo</t>
   </si>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
@@ -394,6 +394,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1400,7 +1401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012D4005-2E5B-4316-B331-8FBB6649AB07}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -1478,7 +1479,7 @@
       <c r="I2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="J2" t="n" s="23">
+      <c r="J2" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1570,7 +1571,7 @@
       <c r="I5" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="J5" t="n" s="23">
+      <c r="J5" t="n" s="24">
         <v>45838.0</v>
       </c>
     </row>
@@ -1602,7 +1603,7 @@
       <c r="I6" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="J6" t="n" s="23">
+      <c r="J6" t="n" s="24">
         <v>46387.0</v>
       </c>
     </row>
@@ -1664,7 +1665,7 @@
       <c r="I8" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J8" t="n" s="23">
+      <c r="J8" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1696,7 +1697,7 @@
       <c r="I9" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J9" t="n" s="23">
+      <c r="J9" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1728,7 +1729,7 @@
       <c r="I10" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J10" t="n" s="23">
+      <c r="J10" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1760,7 +1761,7 @@
       <c r="I11" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J11" t="n" s="23">
+      <c r="J11" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1792,7 +1793,7 @@
       <c r="I12" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J12" t="n" s="23">
+      <c r="J12" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1824,7 +1825,7 @@
       <c r="I13" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J13" t="n" s="23">
+      <c r="J13" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1856,7 +1857,7 @@
       <c r="I14" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J14" t="n" s="23">
+      <c r="J14" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1888,7 +1889,7 @@
       <c r="I15" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J15" t="n" s="23">
+      <c r="J15" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1920,7 +1921,7 @@
       <c r="I16" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J16" t="n" s="23">
+      <c r="J16" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1952,7 +1953,7 @@
       <c r="I17" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J17" t="n" s="23">
+      <c r="J17" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -1984,7 +1985,7 @@
       <c r="I18" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J18" t="n" s="23">
+      <c r="J18" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2016,7 +2017,7 @@
       <c r="I19" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J19" t="n" s="23">
+      <c r="J19" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2048,7 +2049,7 @@
       <c r="I20" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J20" t="n" s="23">
+      <c r="J20" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2080,7 +2081,7 @@
       <c r="I21" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J21" t="n" s="23">
+      <c r="J21" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2112,7 +2113,7 @@
       <c r="I22" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J22" t="n" s="23">
+      <c r="J22" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2144,7 +2145,7 @@
       <c r="I23" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J23" t="n" s="23">
+      <c r="J23" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2176,7 +2177,7 @@
       <c r="I24" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J24" t="n" s="23">
+      <c r="J24" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2208,7 +2209,7 @@
       <c r="I25" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J25" t="n" s="23">
+      <c r="J25" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2240,7 +2241,7 @@
       <c r="I26" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J26" t="n" s="23">
+      <c r="J26" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2272,7 +2273,7 @@
       <c r="I27" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J27" t="n" s="23">
+      <c r="J27" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2304,7 +2305,7 @@
       <c r="I28" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J28" t="n" s="23">
+      <c r="J28" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2336,7 +2337,7 @@
       <c r="I29" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J29" t="n" s="23">
+      <c r="J29" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2368,7 +2369,39 @@
       <c r="I30" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="J30" t="n" s="23">
+      <c r="J30" t="n" s="24">
+        <v>46022.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D31" t="n" s="0">
+        <v>99.39</v>
+      </c>
+      <c r="E31" t="n" s="0">
+        <v>101.2</v>
+      </c>
+      <c r="F31" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="G31" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J31" t="n" s="24">
         <v>46022.0</v>
       </c>
     </row>
@@ -2640,7 +2673,7 @@
       <c r="A2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B2" t="n" s="23">
+      <c r="B2" t="n" s="24">
         <v>45951.0</v>
       </c>
       <c r="C2" t="s" s="0">
@@ -2660,7 +2693,7 @@
       <c r="A3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B3" t="n" s="23">
+      <c r="B3" t="n" s="24">
         <v>45951.0</v>
       </c>
       <c r="C3" t="s" s="0">

</xml_diff>